<commit_message>
Fixed Procedure to STU3 and added missing valuesets
</commit_message>
<xml_diff>
--- a/Mappings/Procedure - STU3.xlsx
+++ b/Mappings/Procedure - STU3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -99,9 +99,6 @@
     <t>RF</t>
   </si>
   <si>
-    <t>Procedure.performedPeriod</t>
-  </si>
-  <si>
     <t>Procedure.bodySite</t>
   </si>
   <si>
@@ -117,15 +114,6 @@
     <t>Procedure.performer.actor</t>
   </si>
   <si>
-    <t>Referenced to ZIB OverdrachtConcern</t>
-  </si>
-  <si>
-    <t>Fits</t>
-  </si>
-  <si>
-    <t>Reference to ZIB MedischHulpmiddel</t>
-  </si>
-  <si>
     <t>VerrichtingAnatomischeLocatieCodelijst</t>
   </si>
   <si>
@@ -168,49 +156,19 @@
     <t>2.16.840.1.113883.2.4.3.120.5.2</t>
   </si>
   <si>
-    <t>Procedure changes a lot with STU3.</t>
-  </si>
-  <si>
     <t>Procedure.extension</t>
   </si>
   <si>
-    <t xml:space="preserve">ZIB valueset binding op Extensible. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slicing based on a @profile discriminator </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension  named Requestor. </t>
-  </si>
-  <si>
-    <t>08-02-2017 Notion made of the translation of Zorgverlener AND Zorgaanbieder to HealthCareProvider</t>
-  </si>
-  <si>
-    <t>08-02-2017 Example does not contain the RequestBy extension (yet).</t>
-  </si>
-  <si>
-    <t>08-02-2017: ZIB-549 -- New translations that will come with the new ZIB publication</t>
-  </si>
-  <si>
-    <t>STU3</t>
-  </si>
-  <si>
-    <t>Additional adjustments:</t>
-  </si>
-  <si>
-    <t>Procedure.basedOn -&gt; set reference constrains</t>
-  </si>
-  <si>
-    <t>Procedure.context -&gt; set reference constrains</t>
-  </si>
-  <si>
-    <t>Procedure.partOf -&gt; set reference constrains</t>
-  </si>
-  <si>
-    <t>Still need an extension</t>
-  </si>
-  <si>
-    <t>Gforge ticket #13159</t>
+    <t>Still need an extension  / Or will procedureRequest be sufficient?</t>
+  </si>
+  <si>
+    <t>Procedure.performedPeriod.start</t>
+  </si>
+  <si>
+    <t>Procedure.performedPeriod.end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current valueset misses valid OID for system. ZIBs 3.0 has fixed the issue. </t>
   </si>
 </sst>
 </file>
@@ -259,10 +217,9 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Open Sans"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -474,7 +431,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -560,9 +517,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
@@ -581,8 +535,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -887,17 +841,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="8" max="8" width="21.28515625" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" customWidth="1"/>
-    <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" customWidth="1"/>
     <col min="11" max="11" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -905,15 +859,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
@@ -926,22 +880,22 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3"/>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="37"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="36"/>
       <c r="J2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="25.5">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -960,13 +914,11 @@
         <v>24</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>48</v>
+      </c>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:11" ht="25.5">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -985,11 +937,9 @@
         <v>24</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>34</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="12">
@@ -1010,11 +960,9 @@
         <v>25</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>34</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="K5" s="23"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="12">
@@ -1034,11 +982,9 @@
         <v>26</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>33</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="21">
@@ -1059,10 +1005,10 @@
         <v>25</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>52</v>
+        <v>29</v>
+      </c>
+      <c r="K7" s="37" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="25.5">
@@ -1084,11 +1030,9 @@
         <v>26</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>35</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="K8" s="20"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="12">
@@ -1109,11 +1053,9 @@
         <v>26</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>53</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="21">
@@ -1134,11 +1076,9 @@
         <v>26</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="20" t="s">
-        <v>53</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="28">
@@ -1159,335 +1099,28 @@
         <v>26</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="K13" s="31" t="s">
-        <v>50</v>
-      </c>
+      <c r="B13" s="30"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="K14" s="31" t="s">
-        <v>56</v>
-      </c>
+      <c r="A14" s="19"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="K15" t="s">
-        <v>55</v>
-      </c>
+      <c r="A15" s="19"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="K16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75">
-      <c r="A19" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="3"/>
-      <c r="B21" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="5">
-        <v>1</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K22" s="11"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="12">
-        <v>2</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" s="17"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="12">
-        <v>3</v>
-      </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="18"/>
-      <c r="I24" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="K24" s="23"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="12">
-        <v>4</v>
-      </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="15"/>
-      <c r="G25" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="16"/>
-      <c r="I25" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="K25" s="20"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="21">
-        <v>5</v>
-      </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="K26" s="23"/>
-    </row>
-    <row r="27" spans="1:11" ht="25.5">
-      <c r="A27" s="21">
-        <v>6</v>
-      </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="K27" s="20"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="12">
-        <v>7</v>
-      </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" s="16"/>
-      <c r="I28" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="K28" s="20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="21">
-        <v>8</v>
-      </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" s="16"/>
-      <c r="I29" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="K29" s="20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="28">
-        <v>10</v>
-      </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="27"/>
-      <c r="I30" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="J30" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="K30" s="29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="B32" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="19">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="19">
-        <v>2</v>
-      </c>
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="19">
-        <v>3</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
+      <c r="A16" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="2">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="A19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1499,7 +1132,7 @@
   <dimension ref="B3:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1511,37 +1144,37 @@
   <sheetData>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1567,32 +1200,32 @@
   <sheetData>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>